<commit_message>
Add 2019 data to the empty spaces heatmap.
</commit_message>
<xml_diff>
--- a/excel_data/2019_data/Win19_wk2_A.xlsx
+++ b/excel_data/2019_data/Win19_wk2_A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Documents\UCSD_old_laptop\Fall_2019\ECE 143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iaman\Desktop\Projects\Project 2019.9\ECE143\Project\ECE143_FinalProject\excel_data\2019_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90612E47-DA3B-43E0-9285-EB2BEA613F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA4EC8-E7FF-46F5-A744-A47D75CFDCA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{FA4123A2-8BA4-4030-9F53-196C65BE7F54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA4123A2-8BA4-4030-9F53-196C65BE7F54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,11 +476,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -493,6 +493,8 @@
     <font>
       <sz val="7"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="7"/>
@@ -507,6 +509,13 @@
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -911,7 +920,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -927,7 +936,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1225,13 +1234,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230AF52D-F3B1-479A-ADCF-BE901E42E4E5}">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1311,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1380,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="17.399999999999999">
+    <row r="3" spans="1:23" ht="21.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1451,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="17.399999999999999">
+    <row r="4" spans="1:23" ht="21.6" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="17.399999999999999">
+    <row r="5" spans="1:23" ht="21.6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>36</v>
       </c>
@@ -1724,7 +1733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.399999999999999">
+    <row r="8" spans="1:23" ht="21.6" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>39</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="21" t="s">
         <v>10</v>
@@ -1864,7 +1873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="11" t="s">
         <v>11</v>
@@ -1933,7 +1942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="21" t="s">
         <v>12</v>
@@ -2002,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="11" t="s">
         <v>13</v>
@@ -2071,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="21" t="s">
         <v>14</v>
@@ -2140,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="11" t="s">
         <v>15</v>
@@ -2209,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="21" t="s">
         <v>16</v>
@@ -2278,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
       <c r="B16" s="11" t="s">
         <v>16</v>
@@ -2347,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="21" t="s">
         <v>17</v>
@@ -2416,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="11" t="s">
         <v>18</v>
@@ -2485,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="21" t="s">
         <v>19</v>
@@ -2554,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="11" t="s">
         <v>19</v>
@@ -2623,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="21" t="s">
         <v>20</v>
@@ -2692,7 +2701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="11" t="s">
         <v>21</v>
@@ -2761,7 +2770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="21" t="s">
         <v>22</v>
@@ -2830,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="11" t="s">
         <v>23</v>
@@ -2899,7 +2908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="21" t="s">
         <v>24</v>
@@ -2968,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="11" t="s">
         <v>25</v>
@@ -3037,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="21" t="s">
         <v>26</v>
@@ -3106,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="11" t="s">
         <v>27</v>
@@ -3175,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
@@ -3244,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
       <c r="B30" s="11" t="s">
         <v>29</v>
@@ -3313,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" s="21" t="s">
         <v>30</v>
@@ -3382,7 +3391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="36"/>
       <c r="B32" s="11" t="s">
         <v>31</v>
@@ -3451,7 +3460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" s="21" t="s">
         <v>31</v>
@@ -3520,7 +3529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="11" t="s">
         <v>32</v>
@@ -3589,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="37"/>
       <c r="B35" s="21" t="s">
         <v>33</v>
@@ -3658,7 +3667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="36"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
@@ -3727,7 +3736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="50" t="s">
         <v>35</v>
@@ -3797,6 +3806,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>